<commit_message>
working on artillery, wrong rotation of artillery and anti air craft fixed
</commit_message>
<xml_diff>
--- a/SeaWar info/تجهیزات متداول.xlsx
+++ b/SeaWar info/تجهیزات متداول.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71772AFA-601E-4189-8154-0848A9BF0387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E56779B-1B79-4CE0-9560-9A087E5791D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L62" sqref="L62"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>

</xml_diff>